<commit_message>
update script to include glossary page
</commit_message>
<xml_diff>
--- a/master_sheet.xlsx
+++ b/master_sheet.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Glossary" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -605,115 +606,119 @@
       </c>
       <c r="AH1" s="1" t="inlineStr">
         <is>
+          <t>Parameter</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
           <t>Baseline</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>Actual</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>Forecast</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>Incident Category</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>Number of Incidents (To-Date)</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>Number of Investigations in Progress</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>Number of Investigations Completed</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>Number of Investigations Pending Approval</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>Audits/Inspections</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>In Progress_audits</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>Completed_audits</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>Remaining Planned</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>Actions</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>In Progress_actions</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>Completed_actions</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>Pending Approval</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>Year</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>Value_training</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>Program</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>Acquired (Ha)</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>Under Negotiation (Ha)</t>
         </is>
       </c>
-      <c r="BC1" s="1" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>Pending (Ha)</t>
         </is>
       </c>
-      <c r="BD1" s="1" t="inlineStr"/>
       <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>Assessment Criteria</t>
@@ -997,22 +1002,24 @@
       <c r="AG2" t="n">
         <v>180</v>
       </c>
-      <c r="AH2" t="n">
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="AI2" t="n">
         <v>186</v>
       </c>
-      <c r="AI2" t="n">
+      <c r="AJ2" t="n">
         <v>129</v>
       </c>
-      <c r="AJ2" t="n">
+      <c r="AK2" t="n">
         <v>50</v>
       </c>
-      <c r="AK2" t="inlineStr">
+      <c r="AL2" t="inlineStr">
         <is>
           <t>Fatalities</t>
         </is>
-      </c>
-      <c r="AL2" t="n">
-        <v>0</v>
       </c>
       <c r="AM2" t="n">
         <v>0</v>
@@ -1023,57 +1030,59 @@
       <c r="AO2" t="n">
         <v>0</v>
       </c>
-      <c r="AP2" t="inlineStr">
+      <c r="AP2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ2" t="inlineStr">
         <is>
           <t>HSE Audit</t>
         </is>
       </c>
-      <c r="AQ2" t="n">
+      <c r="AR2" t="n">
         <v>3</v>
       </c>
-      <c r="AR2" t="n">
+      <c r="AS2" t="n">
         <v>5</v>
       </c>
-      <c r="AS2" t="n">
+      <c r="AT2" t="n">
         <v>4</v>
       </c>
-      <c r="AT2" t="inlineStr">
+      <c r="AU2" t="inlineStr">
         <is>
           <t>HSE</t>
         </is>
       </c>
-      <c r="AU2" t="n">
+      <c r="AV2" t="n">
         <v>6</v>
       </c>
-      <c r="AV2" t="n">
+      <c r="AW2" t="n">
         <v>22</v>
       </c>
-      <c r="AW2" t="n">
+      <c r="AX2" t="n">
         <v>12</v>
       </c>
-      <c r="AX2" t="inlineStr">
+      <c r="AY2" t="inlineStr">
         <is>
           <t>Jan</t>
         </is>
       </c>
-      <c r="AY2" t="n">
+      <c r="AZ2" t="n">
         <v>30</v>
       </c>
-      <c r="AZ2" t="inlineStr">
+      <c r="BA2" t="inlineStr">
         <is>
           <t>Program 1</t>
         </is>
       </c>
-      <c r="BA2" t="n">
+      <c r="BB2" t="n">
         <v>50</v>
       </c>
-      <c r="BB2" t="n">
+      <c r="BC2" t="n">
         <v>25</v>
       </c>
-      <c r="BC2" t="n">
+      <c r="BD2" t="n">
         <v>5</v>
       </c>
-      <c r="BD2" t="inlineStr"/>
       <c r="BE2" t="inlineStr">
         <is>
           <t>% of CESMP mitigation measures which align with ESIA*</t>
@@ -1317,83 +1326,87 @@
       <c r="AG3" t="n">
         <v>120</v>
       </c>
-      <c r="AH3" t="n">
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="AI3" t="n">
         <v>16100</v>
       </c>
-      <c r="AI3" t="n">
+      <c r="AJ3" t="n">
         <v>9600</v>
       </c>
-      <c r="AJ3" t="n">
+      <c r="AK3" t="n">
         <v>6800</v>
       </c>
-      <c r="AK3" t="inlineStr">
+      <c r="AL3" t="inlineStr">
         <is>
           <t>Severe Impairment</t>
         </is>
       </c>
-      <c r="AL3" t="n">
+      <c r="AM3" t="n">
         <v>1</v>
       </c>
-      <c r="AM3" t="n">
+      <c r="AN3" t="n">
         <v>0</v>
       </c>
-      <c r="AN3" t="n">
+      <c r="AO3" t="n">
         <v>1</v>
       </c>
-      <c r="AO3" t="n">
+      <c r="AP3" t="n">
         <v>0</v>
       </c>
-      <c r="AP3" t="inlineStr">
+      <c r="AQ3" t="inlineStr">
         <is>
           <t>Welfare Inspection</t>
         </is>
       </c>
-      <c r="AQ3" t="n">
+      <c r="AR3" t="n">
         <v>2</v>
-      </c>
-      <c r="AR3" t="n">
-        <v>4</v>
       </c>
       <c r="AS3" t="n">
         <v>4</v>
       </c>
-      <c r="AT3" t="inlineStr">
+      <c r="AT3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AU3" t="inlineStr">
         <is>
           <t>Welfare</t>
         </is>
       </c>
-      <c r="AU3" t="n">
+      <c r="AV3" t="n">
         <v>25</v>
       </c>
-      <c r="AV3" t="n">
+      <c r="AW3" t="n">
         <v>10</v>
       </c>
-      <c r="AW3" t="n">
+      <c r="AX3" t="n">
         <v>7</v>
       </c>
-      <c r="AX3" t="inlineStr">
+      <c r="AY3" t="inlineStr">
         <is>
           <t>Feb</t>
         </is>
       </c>
-      <c r="AY3" t="n">
+      <c r="AZ3" t="n">
         <v>40</v>
       </c>
-      <c r="AZ3" t="inlineStr">
+      <c r="BA3" t="inlineStr">
         <is>
           <t>Program 2</t>
         </is>
       </c>
-      <c r="BA3" t="n">
+      <c r="BB3" t="n">
         <v>230</v>
       </c>
-      <c r="BB3" t="n">
+      <c r="BC3" t="n">
         <v>40</v>
       </c>
-      <c r="BC3" t="n">
+      <c r="BD3" t="n">
         <v>30</v>
       </c>
-      <c r="BD3" t="inlineStr"/>
       <c r="BE3" t="inlineStr"/>
       <c r="BF3" t="inlineStr"/>
       <c r="BG3" t="inlineStr"/>
@@ -1602,24 +1615,24 @@
       <c r="AH4" t="inlineStr"/>
       <c r="AI4" t="inlineStr"/>
       <c r="AJ4" t="inlineStr"/>
-      <c r="AK4" t="inlineStr">
+      <c r="AK4" t="inlineStr"/>
+      <c r="AL4" t="inlineStr">
         <is>
           <t>Lost Time Incidents</t>
         </is>
       </c>
-      <c r="AL4" t="n">
+      <c r="AM4" t="n">
         <v>3</v>
       </c>
-      <c r="AM4" t="n">
+      <c r="AN4" t="n">
         <v>0</v>
       </c>
-      <c r="AN4" t="n">
+      <c r="AO4" t="n">
         <v>1</v>
       </c>
-      <c r="AO4" t="n">
+      <c r="AP4" t="n">
         <v>2</v>
       </c>
-      <c r="AP4" t="inlineStr"/>
       <c r="AQ4" t="inlineStr"/>
       <c r="AR4" t="inlineStr"/>
       <c r="AS4" t="inlineStr"/>
@@ -1627,29 +1640,29 @@
       <c r="AU4" t="inlineStr"/>
       <c r="AV4" t="inlineStr"/>
       <c r="AW4" t="inlineStr"/>
-      <c r="AX4" t="inlineStr">
+      <c r="AX4" t="inlineStr"/>
+      <c r="AY4" t="inlineStr">
         <is>
           <t>Mar</t>
         </is>
       </c>
-      <c r="AY4" t="n">
+      <c r="AZ4" t="n">
         <v>38</v>
       </c>
-      <c r="AZ4" t="inlineStr">
+      <c r="BA4" t="inlineStr">
         <is>
           <t>Program 3</t>
         </is>
       </c>
-      <c r="BA4" t="n">
+      <c r="BB4" t="n">
         <v>10</v>
       </c>
-      <c r="BB4" t="n">
+      <c r="BC4" t="n">
         <v>80</v>
       </c>
-      <c r="BC4" t="n">
+      <c r="BD4" t="n">
         <v>10</v>
       </c>
-      <c r="BD4" t="inlineStr"/>
       <c r="BE4" t="inlineStr">
         <is>
           <t>Has the Construction Execution Plan been updated to reflect the latest stage of construction?</t>
@@ -1868,24 +1881,24 @@
       <c r="AH5" t="inlineStr"/>
       <c r="AI5" t="inlineStr"/>
       <c r="AJ5" t="inlineStr"/>
-      <c r="AK5" t="inlineStr">
+      <c r="AK5" t="inlineStr"/>
+      <c r="AL5" t="inlineStr">
         <is>
           <t>Recordable Incidents</t>
         </is>
       </c>
-      <c r="AL5" t="n">
+      <c r="AM5" t="n">
         <v>14</v>
       </c>
-      <c r="AM5" t="n">
+      <c r="AN5" t="n">
         <v>3</v>
       </c>
-      <c r="AN5" t="n">
+      <c r="AO5" t="n">
         <v>11</v>
       </c>
-      <c r="AO5" t="n">
+      <c r="AP5" t="n">
         <v>0</v>
       </c>
-      <c r="AP5" t="inlineStr"/>
       <c r="AQ5" t="inlineStr"/>
       <c r="AR5" t="inlineStr"/>
       <c r="AS5" t="inlineStr"/>
@@ -1893,15 +1906,15 @@
       <c r="AU5" t="inlineStr"/>
       <c r="AV5" t="inlineStr"/>
       <c r="AW5" t="inlineStr"/>
-      <c r="AX5" t="inlineStr">
+      <c r="AX5" t="inlineStr"/>
+      <c r="AY5" t="inlineStr">
         <is>
           <t>Apr</t>
         </is>
       </c>
-      <c r="AY5" t="n">
+      <c r="AZ5" t="n">
         <v>35</v>
       </c>
-      <c r="AZ5" t="inlineStr"/>
       <c r="BA5" t="inlineStr"/>
       <c r="BB5" t="inlineStr"/>
       <c r="BC5" t="inlineStr"/>
@@ -2140,24 +2153,24 @@
       <c r="AH6" t="inlineStr"/>
       <c r="AI6" t="inlineStr"/>
       <c r="AJ6" t="inlineStr"/>
-      <c r="AK6" t="inlineStr">
+      <c r="AK6" t="inlineStr"/>
+      <c r="AL6" t="inlineStr">
         <is>
           <t>Near Misses</t>
         </is>
       </c>
-      <c r="AL6" t="n">
+      <c r="AM6" t="n">
         <v>26</v>
       </c>
-      <c r="AM6" t="n">
+      <c r="AN6" t="n">
         <v>2</v>
       </c>
-      <c r="AN6" t="n">
+      <c r="AO6" t="n">
         <v>21</v>
       </c>
-      <c r="AO6" t="n">
+      <c r="AP6" t="n">
         <v>3</v>
       </c>
-      <c r="AP6" t="inlineStr"/>
       <c r="AQ6" t="inlineStr"/>
       <c r="AR6" t="inlineStr"/>
       <c r="AS6" t="inlineStr"/>
@@ -2165,15 +2178,15 @@
       <c r="AU6" t="inlineStr"/>
       <c r="AV6" t="inlineStr"/>
       <c r="AW6" t="inlineStr"/>
-      <c r="AX6" t="inlineStr">
+      <c r="AX6" t="inlineStr"/>
+      <c r="AY6" t="inlineStr">
         <is>
           <t>May</t>
         </is>
       </c>
-      <c r="AY6" t="n">
+      <c r="AZ6" t="n">
         <v>0</v>
       </c>
-      <c r="AZ6" t="inlineStr"/>
       <c r="BA6" t="inlineStr"/>
       <c r="BB6" t="inlineStr"/>
       <c r="BC6" t="inlineStr"/>
@@ -2401,15 +2414,15 @@
       <c r="AU7" t="inlineStr"/>
       <c r="AV7" t="inlineStr"/>
       <c r="AW7" t="inlineStr"/>
-      <c r="AX7" t="inlineStr">
+      <c r="AX7" t="inlineStr"/>
+      <c r="AY7" t="inlineStr">
         <is>
           <t>Jun</t>
         </is>
       </c>
-      <c r="AY7" t="n">
+      <c r="AZ7" t="n">
         <v>0</v>
       </c>
-      <c r="AZ7" t="inlineStr"/>
       <c r="BA7" t="inlineStr"/>
       <c r="BB7" t="inlineStr"/>
       <c r="BC7" t="inlineStr"/>
@@ -2615,15 +2628,15 @@
       <c r="AU8" t="inlineStr"/>
       <c r="AV8" t="inlineStr"/>
       <c r="AW8" t="inlineStr"/>
-      <c r="AX8" t="inlineStr">
+      <c r="AX8" t="inlineStr"/>
+      <c r="AY8" t="inlineStr">
         <is>
           <t>Jul</t>
         </is>
       </c>
-      <c r="AY8" t="n">
+      <c r="AZ8" t="n">
         <v>0</v>
       </c>
-      <c r="AZ8" t="inlineStr"/>
       <c r="BA8" t="inlineStr"/>
       <c r="BB8" t="inlineStr"/>
       <c r="BC8" t="inlineStr"/>
@@ -2825,15 +2838,15 @@
       <c r="AU9" t="inlineStr"/>
       <c r="AV9" t="inlineStr"/>
       <c r="AW9" t="inlineStr"/>
-      <c r="AX9" t="inlineStr">
+      <c r="AX9" t="inlineStr"/>
+      <c r="AY9" t="inlineStr">
         <is>
           <t>Aug</t>
         </is>
       </c>
-      <c r="AY9" t="n">
+      <c r="AZ9" t="n">
         <v>0</v>
       </c>
-      <c r="AZ9" t="inlineStr"/>
       <c r="BA9" t="inlineStr"/>
       <c r="BB9" t="inlineStr"/>
       <c r="BC9" t="inlineStr"/>
@@ -3047,15 +3060,15 @@
       <c r="AU10" t="inlineStr"/>
       <c r="AV10" t="inlineStr"/>
       <c r="AW10" t="inlineStr"/>
-      <c r="AX10" t="inlineStr">
+      <c r="AX10" t="inlineStr"/>
+      <c r="AY10" t="inlineStr">
         <is>
           <t>Sep</t>
         </is>
       </c>
-      <c r="AY10" t="n">
+      <c r="AZ10" t="n">
         <v>0</v>
       </c>
-      <c r="AZ10" t="inlineStr"/>
       <c r="BA10" t="inlineStr"/>
       <c r="BB10" t="inlineStr"/>
       <c r="BC10" t="inlineStr"/>
@@ -3267,15 +3280,15 @@
       <c r="AU11" t="inlineStr"/>
       <c r="AV11" t="inlineStr"/>
       <c r="AW11" t="inlineStr"/>
-      <c r="AX11" t="inlineStr">
+      <c r="AX11" t="inlineStr"/>
+      <c r="AY11" t="inlineStr">
         <is>
           <t>Oct</t>
         </is>
       </c>
-      <c r="AY11" t="n">
+      <c r="AZ11" t="n">
         <v>0</v>
       </c>
-      <c r="AZ11" t="inlineStr"/>
       <c r="BA11" t="inlineStr"/>
       <c r="BB11" t="inlineStr"/>
       <c r="BC11" t="inlineStr"/>
@@ -3429,15 +3442,15 @@
       <c r="AU12" t="inlineStr"/>
       <c r="AV12" t="inlineStr"/>
       <c r="AW12" t="inlineStr"/>
-      <c r="AX12" t="inlineStr">
+      <c r="AX12" t="inlineStr"/>
+      <c r="AY12" t="inlineStr">
         <is>
           <t>Nov</t>
         </is>
       </c>
-      <c r="AY12" t="n">
+      <c r="AZ12" t="n">
         <v>0</v>
       </c>
-      <c r="AZ12" t="inlineStr"/>
       <c r="BA12" t="inlineStr"/>
       <c r="BB12" t="inlineStr"/>
       <c r="BC12" t="inlineStr"/>
@@ -3611,15 +3624,15 @@
       <c r="AU13" t="inlineStr"/>
       <c r="AV13" t="inlineStr"/>
       <c r="AW13" t="inlineStr"/>
-      <c r="AX13" t="inlineStr">
+      <c r="AX13" t="inlineStr"/>
+      <c r="AY13" t="inlineStr">
         <is>
           <t>Dec</t>
         </is>
       </c>
-      <c r="AY13" t="n">
+      <c r="AZ13" t="n">
         <v>0</v>
       </c>
-      <c r="AZ13" t="inlineStr"/>
       <c r="BA13" t="inlineStr"/>
       <c r="BB13" t="inlineStr"/>
       <c r="BC13" t="inlineStr"/>
@@ -4244,9 +4257,7 @@
           <t>Average time to complete shop drawing reviews</t>
         </is>
       </c>
-      <c r="AG17" t="n">
-        <v>480</v>
-      </c>
+      <c r="AG17" t="inlineStr"/>
       <c r="AH17" t="inlineStr"/>
       <c r="AI17" t="inlineStr"/>
       <c r="AJ17" t="inlineStr"/>
@@ -4386,7 +4397,9 @@
           <t>Number of shop drawing review conducted</t>
         </is>
       </c>
-      <c r="AG18" t="inlineStr"/>
+      <c r="AG18" t="n">
+        <v>14550</v>
+      </c>
       <c r="AH18" t="inlineStr"/>
       <c r="AI18" t="inlineStr"/>
       <c r="AJ18" t="inlineStr"/>
@@ -5278,7 +5291,7 @@
       </c>
       <c r="BK24" t="inlineStr">
         <is>
-          <t>Number of As-Built review requests</t>
+          <t>Number of As-Built Drawing review requests</t>
         </is>
       </c>
       <c r="BL24" t="n">
@@ -5412,7 +5425,7 @@
       <c r="BJ25" t="inlineStr"/>
       <c r="BK25" t="inlineStr">
         <is>
-          <t>Number of As-built reviews / approvals</t>
+          <t>Number of As-Built Drawings reviews approved</t>
         </is>
       </c>
       <c r="BL25" t="n">
@@ -5822,7 +5835,7 @@
       </c>
       <c r="BK28" t="inlineStr">
         <is>
-          <t>Total number of MIRs approved / rejected</t>
+          <t>Total number of MIRs approved</t>
         </is>
       </c>
       <c r="BL28" t="n">
@@ -5922,7 +5935,11 @@
           <t xml:space="preserve">Leadership engagement </t>
         </is>
       </c>
-      <c r="AG29" t="inlineStr"/>
+      <c r="AG29" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
       <c r="AH29" t="inlineStr"/>
       <c r="AI29" t="inlineStr"/>
       <c r="AJ29" t="inlineStr"/>
@@ -6057,13 +6074,11 @@
       <c r="AE30" t="inlineStr"/>
       <c r="AF30" t="inlineStr">
         <is>
-          <t xml:space="preserve">Leadership engagement </t>
-        </is>
-      </c>
-      <c r="AG30" t="inlineStr">
-        <is>
-          <t>Satisfactory</t>
-        </is>
+          <t>Total number of ITPs requested</t>
+        </is>
+      </c>
+      <c r="AG30" t="n">
+        <v>100</v>
       </c>
       <c r="AH30" t="inlineStr"/>
       <c r="AI30" t="inlineStr"/>
@@ -6179,11 +6194,11 @@
       <c r="AE31" t="inlineStr"/>
       <c r="AF31" t="inlineStr">
         <is>
-          <t>Total number of ITPs requested</t>
+          <t>Total number of ITPs attended</t>
         </is>
       </c>
       <c r="AG31" t="n">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="AH31" t="inlineStr"/>
       <c r="AI31" t="inlineStr"/>
@@ -6230,7 +6245,7 @@
       </c>
       <c r="BK31" t="inlineStr">
         <is>
-          <t>Total number of WIRs approved / rejected</t>
+          <t>Total number of WIRs approved</t>
         </is>
       </c>
       <c r="BL31" t="n">
@@ -6303,11 +6318,11 @@
       <c r="AE32" t="inlineStr"/>
       <c r="AF32" t="inlineStr">
         <is>
-          <t>Total number of ITPs attended</t>
+          <t>Total number of ITPs approved</t>
         </is>
       </c>
       <c r="AG32" t="n">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="AH32" t="inlineStr"/>
       <c r="AI32" t="inlineStr"/>
@@ -6467,11 +6482,11 @@
       <c r="AE33" t="inlineStr"/>
       <c r="AF33" t="inlineStr">
         <is>
-          <t>Total number of ITPs approved</t>
+          <t>Total number of ITPs completed</t>
         </is>
       </c>
       <c r="AG33" t="n">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="AH33" t="inlineStr"/>
       <c r="AI33" t="inlineStr"/>
@@ -6601,12 +6616,10 @@
       <c r="AE34" t="inlineStr"/>
       <c r="AF34" t="inlineStr">
         <is>
-          <t>Total number of ITPs completed</t>
-        </is>
-      </c>
-      <c r="AG34" t="n">
-        <v>85</v>
-      </c>
+          <t>Total number Quality Reports completed</t>
+        </is>
+      </c>
+      <c r="AG34" t="inlineStr"/>
       <c r="AH34" t="inlineStr"/>
       <c r="AI34" t="inlineStr"/>
       <c r="AJ34" t="inlineStr"/>
@@ -6711,10 +6724,14 @@
       <c r="AE35" t="inlineStr"/>
       <c r="AF35" t="inlineStr">
         <is>
-          <t>Total number Quality Reports completed</t>
-        </is>
-      </c>
-      <c r="AG35" t="inlineStr"/>
+          <t>Completeness of Quality Management Plan</t>
+        </is>
+      </c>
+      <c r="AG35" t="inlineStr">
+        <is>
+          <t>Needs Improvement</t>
+        </is>
+      </c>
       <c r="AH35" t="inlineStr"/>
       <c r="AI35" t="inlineStr"/>
       <c r="AJ35" t="inlineStr"/>
@@ -6847,14 +6864,10 @@
       <c r="AE36" t="inlineStr"/>
       <c r="AF36" t="inlineStr">
         <is>
-          <t>Completeness of Quality Management Plan</t>
-        </is>
-      </c>
-      <c r="AG36" t="inlineStr">
-        <is>
-          <t>Needs Improvement</t>
-        </is>
-      </c>
+          <t>Required number of ITPs signed off throughout construction</t>
+        </is>
+      </c>
+      <c r="AG36" t="inlineStr"/>
       <c r="AH36" t="inlineStr"/>
       <c r="AI36" t="inlineStr"/>
       <c r="AJ36" t="inlineStr"/>
@@ -6999,7 +7012,7 @@
       <c r="AE37" t="inlineStr"/>
       <c r="AF37" t="inlineStr">
         <is>
-          <t>Required number of ITPs signed off throughout construction</t>
+          <t>Total number of raised closed-out defects &amp; NCRs</t>
         </is>
       </c>
       <c r="AG37" t="inlineStr"/>
@@ -7107,7 +7120,7 @@
       <c r="AE38" t="inlineStr"/>
       <c r="AF38" t="inlineStr">
         <is>
-          <t>Total number of raised closed-out defects &amp; NCRs</t>
+          <t>Forecasted Procurement Budget</t>
         </is>
       </c>
       <c r="AG38" t="inlineStr"/>
@@ -7251,7 +7264,7 @@
       <c r="AE39" t="inlineStr"/>
       <c r="AF39" t="inlineStr">
         <is>
-          <t>Forecasted Procurement Budget</t>
+          <t>Actual Procurement Budget</t>
         </is>
       </c>
       <c r="AG39" t="inlineStr"/>
@@ -7359,7 +7372,7 @@
       <c r="AE40" t="inlineStr"/>
       <c r="AF40" t="inlineStr">
         <is>
-          <t>Actual Procurement Budget</t>
+          <t>Vendor Database</t>
         </is>
       </c>
       <c r="AG40" t="inlineStr"/>
@@ -7501,7 +7514,7 @@
       <c r="AE41" t="inlineStr"/>
       <c r="AF41" t="inlineStr">
         <is>
-          <t>Vendor Database</t>
+          <t>Vendor Shortlist</t>
         </is>
       </c>
       <c r="AG41" t="inlineStr"/>
@@ -7603,7 +7616,7 @@
       <c r="AE42" t="inlineStr"/>
       <c r="AF42" t="inlineStr">
         <is>
-          <t>Vendor Shortlist</t>
+          <t>Vendor Awarded</t>
         </is>
       </c>
       <c r="AG42" t="inlineStr"/>
@@ -7719,7 +7732,7 @@
       <c r="AE43" t="inlineStr"/>
       <c r="AF43" t="inlineStr">
         <is>
-          <t>Vendor Awarded</t>
+          <t>Vendor KPIs</t>
         </is>
       </c>
       <c r="AG43" t="inlineStr"/>
@@ -7821,7 +7834,7 @@
       <c r="AE44" t="inlineStr"/>
       <c r="AF44" t="inlineStr">
         <is>
-          <t>Vendor KPIs</t>
+          <t>Vendor Performance Database</t>
         </is>
       </c>
       <c r="AG44" t="inlineStr"/>
@@ -7941,7 +7954,7 @@
       <c r="AE45" t="inlineStr"/>
       <c r="AF45" t="inlineStr">
         <is>
-          <t>Vendor Performance Database</t>
+          <t>Tender return date: Planned / Actual</t>
         </is>
       </c>
       <c r="AG45" t="inlineStr"/>
@@ -8063,7 +8076,7 @@
       <c r="AE46" t="inlineStr"/>
       <c r="AF46" t="inlineStr">
         <is>
-          <t>Tender return date: Planned / Actual</t>
+          <t>Tender Review &amp; award time: Planned / actual</t>
         </is>
       </c>
       <c r="AG46" t="inlineStr"/>
@@ -8165,7 +8178,7 @@
       <c r="AE47" t="inlineStr"/>
       <c r="AF47" t="inlineStr">
         <is>
-          <t>Tender Review &amp; award time: Planned / actual</t>
+          <t>Pre-Tender Cost Estimate</t>
         </is>
       </c>
       <c r="AG47" t="inlineStr"/>
@@ -8281,7 +8294,7 @@
       <c r="AE48" t="inlineStr"/>
       <c r="AF48" t="inlineStr">
         <is>
-          <t>Pre-Tender Cost Estimate</t>
+          <t xml:space="preserve">Tender Performance Index </t>
         </is>
       </c>
       <c r="AG48" t="inlineStr"/>
@@ -8383,10 +8396,14 @@
       <c r="AE49" t="inlineStr"/>
       <c r="AF49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Tender Performance Index </t>
-        </is>
-      </c>
-      <c r="AG49" t="inlineStr"/>
+          <t>Contract clauses</t>
+        </is>
+      </c>
+      <c r="AG49" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
       <c r="AH49" t="inlineStr"/>
       <c r="AI49" t="inlineStr"/>
       <c r="AJ49" t="inlineStr"/>
@@ -8499,12 +8516,12 @@
       <c r="AE50" t="inlineStr"/>
       <c r="AF50" t="inlineStr">
         <is>
-          <t>Contract clauses</t>
+          <t>Procurement Management Plan</t>
         </is>
       </c>
       <c r="AG50" t="inlineStr">
         <is>
-          <t>Satisfactory</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="AH50" t="inlineStr"/>
@@ -8623,12 +8640,12 @@
       <c r="AE51" t="inlineStr"/>
       <c r="AF51" t="inlineStr">
         <is>
-          <t>Procurement Management Plan</t>
+          <t xml:space="preserve">Scope / design maturity </t>
         </is>
       </c>
       <c r="AG51" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Satisfactory</t>
         </is>
       </c>
       <c r="AH51" t="inlineStr"/>
@@ -8747,14 +8764,10 @@
       <c r="AE52" t="inlineStr"/>
       <c r="AF52" t="inlineStr">
         <is>
-          <t xml:space="preserve">Scope / design maturity </t>
-        </is>
-      </c>
-      <c r="AG52" t="inlineStr">
-        <is>
-          <t>Satisfactory</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Compliance with local content regulations / policies </t>
+        </is>
+      </c>
+      <c r="AG52" t="inlineStr"/>
       <c r="AH52" t="inlineStr"/>
       <c r="AI52" t="inlineStr"/>
       <c r="AJ52" t="inlineStr"/>
@@ -8877,7 +8890,7 @@
       <c r="AE53" t="inlineStr"/>
       <c r="AF53" t="inlineStr">
         <is>
-          <t xml:space="preserve">Compliance with local content regulations / policies </t>
+          <t xml:space="preserve">Dispute rate </t>
         </is>
       </c>
       <c r="AG53" t="inlineStr"/>
@@ -8997,7 +9010,7 @@
       <c r="AE54" t="inlineStr"/>
       <c r="AF54" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dispute rate </t>
+          <t xml:space="preserve">Claims processing cycle time </t>
         </is>
       </c>
       <c r="AG54" t="inlineStr"/>
@@ -9113,7 +9126,7 @@
       <c r="AE55" t="inlineStr"/>
       <c r="AF55" t="inlineStr">
         <is>
-          <t xml:space="preserve">Claims processing cycle time </t>
+          <t>No. of related CRs being requested during or after tendering phase due to identified scope gap</t>
         </is>
       </c>
       <c r="AG55" t="inlineStr"/>
@@ -9215,10 +9228,14 @@
       <c r="AE56" t="inlineStr"/>
       <c r="AF56" t="inlineStr">
         <is>
-          <t>No. of related CRs being requested during or after tendering phase due to identified scope gap</t>
-        </is>
-      </c>
-      <c r="AG56" t="inlineStr"/>
+          <t>Vendor Performance Assessment</t>
+        </is>
+      </c>
+      <c r="AG56" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
       <c r="AH56" t="inlineStr"/>
       <c r="AI56" t="inlineStr"/>
       <c r="AJ56" t="inlineStr"/>
@@ -9335,12 +9352,12 @@
       <c r="AE57" t="inlineStr"/>
       <c r="AF57" t="inlineStr">
         <is>
-          <t>Vendor Performance Assessment</t>
+          <t>Tender pack quality</t>
         </is>
       </c>
       <c r="AG57" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Satisfactory</t>
         </is>
       </c>
       <c r="AH57" t="inlineStr"/>
@@ -9455,13 +9472,11 @@
       <c r="AE58" t="inlineStr"/>
       <c r="AF58" t="inlineStr">
         <is>
-          <t>Tender pack quality</t>
-        </is>
-      </c>
-      <c r="AG58" t="inlineStr">
-        <is>
-          <t>Satisfactory</t>
-        </is>
+          <t>% payment paid within contractual terms</t>
+        </is>
+      </c>
+      <c r="AG58" t="n">
+        <v>80</v>
       </c>
       <c r="AH58" t="inlineStr"/>
       <c r="AI58" t="inlineStr"/>
@@ -9561,12 +9576,10 @@
       <c r="AE59" t="inlineStr"/>
       <c r="AF59" t="inlineStr">
         <is>
-          <t>% payment paid within contractual terms</t>
-        </is>
-      </c>
-      <c r="AG59" t="n">
-        <v>80</v>
-      </c>
+          <t>Planned Packages</t>
+        </is>
+      </c>
+      <c r="AG59" t="inlineStr"/>
       <c r="AH59" t="inlineStr"/>
       <c r="AI59" t="inlineStr"/>
       <c r="AJ59" t="inlineStr"/>
@@ -9681,7 +9694,7 @@
       <c r="AE60" t="inlineStr"/>
       <c r="AF60" t="inlineStr">
         <is>
-          <t>Planned Packages</t>
+          <t>Awarded Packages</t>
         </is>
       </c>
       <c r="AG60" t="inlineStr"/>
@@ -9783,7 +9796,7 @@
       <c r="AE61" t="inlineStr"/>
       <c r="AF61" t="inlineStr">
         <is>
-          <t>Awarded Packages</t>
+          <t>Trade Most at Risk</t>
         </is>
       </c>
       <c r="AG61" t="inlineStr"/>
@@ -9887,7 +9900,7 @@
       <c r="AE62" t="inlineStr"/>
       <c r="AF62" t="inlineStr">
         <is>
-          <t>Trade Most at Risk</t>
+          <t xml:space="preserve">Highest Risk Work Site </t>
         </is>
       </c>
       <c r="AG62" t="inlineStr"/>
@@ -9991,7 +10004,7 @@
       <c r="AE63" t="inlineStr"/>
       <c r="AF63" t="inlineStr">
         <is>
-          <t xml:space="preserve">Highest Risk Work Site </t>
+          <t>Number of planned audits</t>
         </is>
       </c>
       <c r="AG63" t="inlineStr"/>
@@ -10107,7 +10120,7 @@
       <c r="AE64" t="inlineStr"/>
       <c r="AF64" t="inlineStr">
         <is>
-          <t>Number of planned audits</t>
+          <t xml:space="preserve">Number of conducted audits </t>
         </is>
       </c>
       <c r="AG64" t="inlineStr"/>
@@ -10223,10 +10236,12 @@
       <c r="AE65" t="inlineStr"/>
       <c r="AF65" t="inlineStr">
         <is>
-          <t xml:space="preserve">Number of conducted audits </t>
-        </is>
-      </c>
-      <c r="AG65" t="inlineStr"/>
+          <t>Number of Notifiable Incidents</t>
+        </is>
+      </c>
+      <c r="AG65" t="n">
+        <v>6</v>
+      </c>
       <c r="AH65" t="inlineStr"/>
       <c r="AI65" t="inlineStr"/>
       <c r="AJ65" t="inlineStr"/>
@@ -10339,11 +10354,11 @@
       <c r="AE66" t="inlineStr"/>
       <c r="AF66" t="inlineStr">
         <is>
-          <t>Number of Notifiable Incidents</t>
+          <t>Number of Infringement Notices</t>
         </is>
       </c>
       <c r="AG66" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AH66" t="inlineStr"/>
       <c r="AI66" t="inlineStr"/>
@@ -10457,12 +10472,10 @@
       <c r="AE67" t="inlineStr"/>
       <c r="AF67" t="inlineStr">
         <is>
-          <t>Number of Infringement Notices</t>
-        </is>
-      </c>
-      <c r="AG67" t="n">
-        <v>2</v>
-      </c>
+          <t xml:space="preserve">Total Safe Manhours </t>
+        </is>
+      </c>
+      <c r="AG67" t="inlineStr"/>
       <c r="AH67" t="inlineStr"/>
       <c r="AI67" t="inlineStr"/>
       <c r="AJ67" t="inlineStr"/>
@@ -10575,7 +10588,7 @@
       <c r="AE68" t="inlineStr"/>
       <c r="AF68" t="inlineStr">
         <is>
-          <t xml:space="preserve">Total Safe Manhours </t>
+          <t xml:space="preserve">Total number of closed Corrective actions </t>
         </is>
       </c>
       <c r="AG68" t="inlineStr"/>
@@ -10691,7 +10704,7 @@
       <c r="AE69" t="inlineStr"/>
       <c r="AF69" t="inlineStr">
         <is>
-          <t xml:space="preserve">Total number of closed Corrective actions </t>
+          <t>Inspection Pass Rate</t>
         </is>
       </c>
       <c r="AG69" t="inlineStr"/>
@@ -10793,7 +10806,7 @@
       <c r="AE70" t="inlineStr"/>
       <c r="AF70" t="inlineStr">
         <is>
-          <t>Inspection Pass Rate</t>
+          <t>No. of recurring incidents / safety observations outside control</t>
         </is>
       </c>
       <c r="AG70" t="inlineStr"/>
@@ -10915,10 +10928,12 @@
       <c r="AE71" t="inlineStr"/>
       <c r="AF71" t="inlineStr">
         <is>
-          <t>No. of recurring incidents / safety observations outside control</t>
-        </is>
-      </c>
-      <c r="AG71" t="inlineStr"/>
+          <t xml:space="preserve">Total Site Manhours </t>
+        </is>
+      </c>
+      <c r="AG71" t="n">
+        <v>180000000</v>
+      </c>
       <c r="AH71" t="inlineStr"/>
       <c r="AI71" t="inlineStr"/>
       <c r="AJ71" t="inlineStr"/>
@@ -11017,12 +11032,10 @@
       <c r="AE72" t="inlineStr"/>
       <c r="AF72" t="inlineStr">
         <is>
-          <t xml:space="preserve">Total Site Manhours </t>
-        </is>
-      </c>
-      <c r="AG72" t="n">
-        <v>180000000</v>
-      </c>
+          <t>Welfare of labor camps</t>
+        </is>
+      </c>
+      <c r="AG72" t="inlineStr"/>
       <c r="AH72" t="inlineStr"/>
       <c r="AI72" t="inlineStr"/>
       <c r="AJ72" t="inlineStr"/>
@@ -11139,7 +11152,7 @@
       <c r="AE73" t="inlineStr"/>
       <c r="AF73" t="inlineStr">
         <is>
-          <t>Welfare of labor camps</t>
+          <t>Welfare of site facilities</t>
         </is>
       </c>
       <c r="AG73" t="inlineStr"/>
@@ -11259,7 +11272,7 @@
       <c r="AE74" t="inlineStr"/>
       <c r="AF74" t="inlineStr">
         <is>
-          <t>Welfare of site facilities</t>
+          <t>Labor accommodation inspection rate</t>
         </is>
       </c>
       <c r="AG74" t="inlineStr"/>
@@ -11375,7 +11388,7 @@
       <c r="AE75" t="inlineStr"/>
       <c r="AF75" t="inlineStr">
         <is>
-          <t>Labor accommodation inspection rate</t>
+          <t xml:space="preserve">Regulation Compliance </t>
         </is>
       </c>
       <c r="AG75" t="inlineStr"/>
@@ -11475,11 +11488,7 @@
       <c r="AC76" t="inlineStr"/>
       <c r="AD76" t="inlineStr"/>
       <c r="AE76" t="inlineStr"/>
-      <c r="AF76" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Regulation Compliance </t>
-        </is>
-      </c>
+      <c r="AF76" t="inlineStr"/>
       <c r="AG76" t="inlineStr"/>
       <c r="AH76" t="inlineStr"/>
       <c r="AI76" t="inlineStr"/>
@@ -12011,22 +12020,24 @@
       <c r="AG80" t="n">
         <v>180</v>
       </c>
-      <c r="AH80" t="n">
+      <c r="AH80" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="AI80" t="n">
         <v>186</v>
       </c>
-      <c r="AI80" t="n">
+      <c r="AJ80" t="n">
         <v>129</v>
       </c>
-      <c r="AJ80" t="n">
+      <c r="AK80" t="n">
         <v>50</v>
       </c>
-      <c r="AK80" t="inlineStr">
+      <c r="AL80" t="inlineStr">
         <is>
           <t>Fatalities</t>
         </is>
-      </c>
-      <c r="AL80" t="n">
-        <v>0</v>
       </c>
       <c r="AM80" t="n">
         <v>0</v>
@@ -12037,57 +12048,59 @@
       <c r="AO80" t="n">
         <v>0</v>
       </c>
-      <c r="AP80" t="inlineStr">
+      <c r="AP80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ80" t="inlineStr">
         <is>
           <t>HSE Audit</t>
         </is>
       </c>
-      <c r="AQ80" t="n">
+      <c r="AR80" t="n">
         <v>3</v>
       </c>
-      <c r="AR80" t="n">
+      <c r="AS80" t="n">
         <v>5</v>
       </c>
-      <c r="AS80" t="n">
+      <c r="AT80" t="n">
         <v>4</v>
       </c>
-      <c r="AT80" t="inlineStr">
+      <c r="AU80" t="inlineStr">
         <is>
           <t>HSE</t>
         </is>
       </c>
-      <c r="AU80" t="n">
+      <c r="AV80" t="n">
         <v>6</v>
       </c>
-      <c r="AV80" t="n">
+      <c r="AW80" t="n">
         <v>22</v>
       </c>
-      <c r="AW80" t="n">
+      <c r="AX80" t="n">
         <v>12</v>
       </c>
-      <c r="AX80" t="inlineStr">
+      <c r="AY80" t="inlineStr">
         <is>
           <t>Jan</t>
         </is>
       </c>
-      <c r="AY80" t="n">
+      <c r="AZ80" t="n">
         <v>30</v>
       </c>
-      <c r="AZ80" t="inlineStr">
+      <c r="BA80" t="inlineStr">
         <is>
           <t>Program 1</t>
         </is>
       </c>
-      <c r="BA80" t="n">
+      <c r="BB80" t="n">
         <v>50</v>
       </c>
-      <c r="BB80" t="n">
+      <c r="BC80" t="n">
         <v>25</v>
       </c>
-      <c r="BC80" t="n">
+      <c r="BD80" t="n">
         <v>20</v>
       </c>
-      <c r="BD80" t="inlineStr"/>
       <c r="BE80" t="inlineStr">
         <is>
           <t>% of CESMP mitigation measures which align with ESIA*</t>
@@ -12317,83 +12330,87 @@
       <c r="AG81" t="n">
         <v>120</v>
       </c>
-      <c r="AH81" t="n">
+      <c r="AH81" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="AI81" t="n">
         <v>16100</v>
       </c>
-      <c r="AI81" t="n">
+      <c r="AJ81" t="n">
         <v>9600</v>
       </c>
-      <c r="AJ81" t="n">
+      <c r="AK81" t="n">
         <v>6800</v>
       </c>
-      <c r="AK81" t="inlineStr">
+      <c r="AL81" t="inlineStr">
         <is>
           <t>Severe Impairment</t>
         </is>
       </c>
-      <c r="AL81" t="n">
+      <c r="AM81" t="n">
         <v>1</v>
       </c>
-      <c r="AM81" t="n">
+      <c r="AN81" t="n">
         <v>0</v>
       </c>
-      <c r="AN81" t="n">
+      <c r="AO81" t="n">
         <v>1</v>
       </c>
-      <c r="AO81" t="n">
+      <c r="AP81" t="n">
         <v>0</v>
       </c>
-      <c r="AP81" t="inlineStr">
+      <c r="AQ81" t="inlineStr">
         <is>
           <t>Welfare Inspection</t>
         </is>
       </c>
-      <c r="AQ81" t="n">
+      <c r="AR81" t="n">
         <v>2</v>
-      </c>
-      <c r="AR81" t="n">
-        <v>4</v>
       </c>
       <c r="AS81" t="n">
         <v>4</v>
       </c>
-      <c r="AT81" t="inlineStr">
+      <c r="AT81" t="n">
+        <v>4</v>
+      </c>
+      <c r="AU81" t="inlineStr">
         <is>
           <t>Welfare</t>
         </is>
       </c>
-      <c r="AU81" t="n">
+      <c r="AV81" t="n">
         <v>25</v>
       </c>
-      <c r="AV81" t="n">
+      <c r="AW81" t="n">
         <v>10</v>
       </c>
-      <c r="AW81" t="n">
+      <c r="AX81" t="n">
         <v>7</v>
       </c>
-      <c r="AX81" t="inlineStr">
+      <c r="AY81" t="inlineStr">
         <is>
           <t>Feb</t>
         </is>
       </c>
-      <c r="AY81" t="n">
+      <c r="AZ81" t="n">
         <v>40</v>
       </c>
-      <c r="AZ81" t="inlineStr">
+      <c r="BA81" t="inlineStr">
         <is>
           <t>Program 2</t>
         </is>
       </c>
-      <c r="BA81" t="n">
+      <c r="BB81" t="n">
         <v>230</v>
       </c>
-      <c r="BB81" t="n">
+      <c r="BC81" t="n">
         <v>40</v>
       </c>
-      <c r="BC81" t="n">
+      <c r="BD81" t="n">
         <v>90</v>
       </c>
-      <c r="BD81" t="inlineStr"/>
       <c r="BE81" t="inlineStr"/>
       <c r="BF81" t="inlineStr"/>
       <c r="BG81" t="inlineStr"/>
@@ -12602,24 +12619,24 @@
       <c r="AH82" t="inlineStr"/>
       <c r="AI82" t="inlineStr"/>
       <c r="AJ82" t="inlineStr"/>
-      <c r="AK82" t="inlineStr">
+      <c r="AK82" t="inlineStr"/>
+      <c r="AL82" t="inlineStr">
         <is>
           <t>Lost Time Incidents</t>
         </is>
       </c>
-      <c r="AL82" t="n">
+      <c r="AM82" t="n">
         <v>3</v>
       </c>
-      <c r="AM82" t="n">
+      <c r="AN82" t="n">
         <v>0</v>
       </c>
-      <c r="AN82" t="n">
+      <c r="AO82" t="n">
         <v>1</v>
       </c>
-      <c r="AO82" t="n">
+      <c r="AP82" t="n">
         <v>2</v>
       </c>
-      <c r="AP82" t="inlineStr"/>
       <c r="AQ82" t="inlineStr"/>
       <c r="AR82" t="inlineStr"/>
       <c r="AS82" t="inlineStr"/>
@@ -12627,29 +12644,29 @@
       <c r="AU82" t="inlineStr"/>
       <c r="AV82" t="inlineStr"/>
       <c r="AW82" t="inlineStr"/>
-      <c r="AX82" t="inlineStr">
+      <c r="AX82" t="inlineStr"/>
+      <c r="AY82" t="inlineStr">
         <is>
           <t>Mar</t>
         </is>
       </c>
-      <c r="AY82" t="n">
+      <c r="AZ82" t="n">
         <v>38</v>
       </c>
-      <c r="AZ82" t="inlineStr">
+      <c r="BA82" t="inlineStr">
         <is>
           <t>Program 3</t>
         </is>
       </c>
-      <c r="BA82" t="n">
+      <c r="BB82" t="n">
         <v>10</v>
       </c>
-      <c r="BB82" t="n">
+      <c r="BC82" t="n">
         <v>80</v>
       </c>
-      <c r="BC82" t="n">
+      <c r="BD82" t="n">
         <v>40</v>
       </c>
-      <c r="BD82" t="inlineStr"/>
       <c r="BE82" t="inlineStr">
         <is>
           <t>Has the Construction Execution Plan been updated to reflect the latest stage of construction?</t>
@@ -12866,24 +12883,24 @@
       <c r="AH83" t="inlineStr"/>
       <c r="AI83" t="inlineStr"/>
       <c r="AJ83" t="inlineStr"/>
-      <c r="AK83" t="inlineStr">
+      <c r="AK83" t="inlineStr"/>
+      <c r="AL83" t="inlineStr">
         <is>
           <t>Recordable Incidents</t>
         </is>
       </c>
-      <c r="AL83" t="n">
+      <c r="AM83" t="n">
         <v>14</v>
       </c>
-      <c r="AM83" t="n">
+      <c r="AN83" t="n">
         <v>3</v>
       </c>
-      <c r="AN83" t="n">
+      <c r="AO83" t="n">
         <v>11</v>
       </c>
-      <c r="AO83" t="n">
+      <c r="AP83" t="n">
         <v>0</v>
       </c>
-      <c r="AP83" t="inlineStr"/>
       <c r="AQ83" t="inlineStr"/>
       <c r="AR83" t="inlineStr"/>
       <c r="AS83" t="inlineStr"/>
@@ -12891,15 +12908,15 @@
       <c r="AU83" t="inlineStr"/>
       <c r="AV83" t="inlineStr"/>
       <c r="AW83" t="inlineStr"/>
-      <c r="AX83" t="inlineStr">
+      <c r="AX83" t="inlineStr"/>
+      <c r="AY83" t="inlineStr">
         <is>
           <t>Apr</t>
         </is>
       </c>
-      <c r="AY83" t="n">
+      <c r="AZ83" t="n">
         <v>35</v>
       </c>
-      <c r="AZ83" t="inlineStr"/>
       <c r="BA83" t="inlineStr"/>
       <c r="BB83" t="inlineStr"/>
       <c r="BC83" t="inlineStr"/>
@@ -13138,24 +13155,24 @@
       <c r="AH84" t="inlineStr"/>
       <c r="AI84" t="inlineStr"/>
       <c r="AJ84" t="inlineStr"/>
-      <c r="AK84" t="inlineStr">
+      <c r="AK84" t="inlineStr"/>
+      <c r="AL84" t="inlineStr">
         <is>
           <t>Nears Misses</t>
         </is>
       </c>
-      <c r="AL84" t="n">
+      <c r="AM84" t="n">
         <v>26</v>
       </c>
-      <c r="AM84" t="n">
+      <c r="AN84" t="n">
         <v>2</v>
       </c>
-      <c r="AN84" t="n">
+      <c r="AO84" t="n">
         <v>21</v>
       </c>
-      <c r="AO84" t="n">
+      <c r="AP84" t="n">
         <v>3</v>
       </c>
-      <c r="AP84" t="inlineStr"/>
       <c r="AQ84" t="inlineStr"/>
       <c r="AR84" t="inlineStr"/>
       <c r="AS84" t="inlineStr"/>
@@ -13163,15 +13180,15 @@
       <c r="AU84" t="inlineStr"/>
       <c r="AV84" t="inlineStr"/>
       <c r="AW84" t="inlineStr"/>
-      <c r="AX84" t="inlineStr">
+      <c r="AX84" t="inlineStr"/>
+      <c r="AY84" t="inlineStr">
         <is>
           <t>May</t>
         </is>
       </c>
-      <c r="AY84" t="n">
+      <c r="AZ84" t="n">
         <v>0</v>
       </c>
-      <c r="AZ84" t="inlineStr"/>
       <c r="BA84" t="inlineStr"/>
       <c r="BB84" t="inlineStr"/>
       <c r="BC84" t="inlineStr"/>
@@ -13403,15 +13420,15 @@
       <c r="AU85" t="inlineStr"/>
       <c r="AV85" t="inlineStr"/>
       <c r="AW85" t="inlineStr"/>
-      <c r="AX85" t="inlineStr">
+      <c r="AX85" t="inlineStr"/>
+      <c r="AY85" t="inlineStr">
         <is>
           <t>Jun</t>
         </is>
       </c>
-      <c r="AY85" t="n">
+      <c r="AZ85" t="n">
         <v>0</v>
       </c>
-      <c r="AZ85" t="inlineStr"/>
       <c r="BA85" t="inlineStr"/>
       <c r="BB85" t="inlineStr"/>
       <c r="BC85" t="inlineStr"/>
@@ -13623,15 +13640,15 @@
       <c r="AU86" t="inlineStr"/>
       <c r="AV86" t="inlineStr"/>
       <c r="AW86" t="inlineStr"/>
-      <c r="AX86" t="inlineStr">
+      <c r="AX86" t="inlineStr"/>
+      <c r="AY86" t="inlineStr">
         <is>
           <t>Jul</t>
         </is>
       </c>
-      <c r="AY86" t="n">
+      <c r="AZ86" t="n">
         <v>0</v>
       </c>
-      <c r="AZ86" t="inlineStr"/>
       <c r="BA86" t="inlineStr"/>
       <c r="BB86" t="inlineStr"/>
       <c r="BC86" t="inlineStr"/>
@@ -13831,15 +13848,15 @@
       <c r="AU87" t="inlineStr"/>
       <c r="AV87" t="inlineStr"/>
       <c r="AW87" t="inlineStr"/>
-      <c r="AX87" t="inlineStr">
+      <c r="AX87" t="inlineStr"/>
+      <c r="AY87" t="inlineStr">
         <is>
           <t>Aug</t>
         </is>
       </c>
-      <c r="AY87" t="n">
+      <c r="AZ87" t="n">
         <v>0</v>
       </c>
-      <c r="AZ87" t="inlineStr"/>
       <c r="BA87" t="inlineStr"/>
       <c r="BB87" t="inlineStr"/>
       <c r="BC87" t="inlineStr"/>
@@ -14053,15 +14070,15 @@
       <c r="AU88" t="inlineStr"/>
       <c r="AV88" t="inlineStr"/>
       <c r="AW88" t="inlineStr"/>
-      <c r="AX88" t="inlineStr">
+      <c r="AX88" t="inlineStr"/>
+      <c r="AY88" t="inlineStr">
         <is>
           <t>Sep</t>
         </is>
       </c>
-      <c r="AY88" t="n">
+      <c r="AZ88" t="n">
         <v>0</v>
       </c>
-      <c r="AZ88" t="inlineStr"/>
       <c r="BA88" t="inlineStr"/>
       <c r="BB88" t="inlineStr"/>
       <c r="BC88" t="inlineStr"/>
@@ -14271,15 +14288,15 @@
       <c r="AU89" t="inlineStr"/>
       <c r="AV89" t="inlineStr"/>
       <c r="AW89" t="inlineStr"/>
-      <c r="AX89" t="inlineStr">
+      <c r="AX89" t="inlineStr"/>
+      <c r="AY89" t="inlineStr">
         <is>
           <t>Oct</t>
         </is>
       </c>
-      <c r="AY89" t="n">
+      <c r="AZ89" t="n">
         <v>0</v>
       </c>
-      <c r="AZ89" t="inlineStr"/>
       <c r="BA89" t="inlineStr"/>
       <c r="BB89" t="inlineStr"/>
       <c r="BC89" t="inlineStr"/>
@@ -14431,15 +14448,15 @@
       <c r="AU90" t="inlineStr"/>
       <c r="AV90" t="inlineStr"/>
       <c r="AW90" t="inlineStr"/>
-      <c r="AX90" t="inlineStr">
+      <c r="AX90" t="inlineStr"/>
+      <c r="AY90" t="inlineStr">
         <is>
           <t>Nov</t>
         </is>
       </c>
-      <c r="AY90" t="n">
+      <c r="AZ90" t="n">
         <v>0</v>
       </c>
-      <c r="AZ90" t="inlineStr"/>
       <c r="BA90" t="inlineStr"/>
       <c r="BB90" t="inlineStr"/>
       <c r="BC90" t="inlineStr"/>
@@ -14611,15 +14628,15 @@
       <c r="AU91" t="inlineStr"/>
       <c r="AV91" t="inlineStr"/>
       <c r="AW91" t="inlineStr"/>
-      <c r="AX91" t="inlineStr">
+      <c r="AX91" t="inlineStr"/>
+      <c r="AY91" t="inlineStr">
         <is>
           <t>Dec</t>
         </is>
       </c>
-      <c r="AY91" t="n">
+      <c r="AZ91" t="n">
         <v>0</v>
       </c>
-      <c r="AZ91" t="inlineStr"/>
       <c r="BA91" t="inlineStr"/>
       <c r="BB91" t="inlineStr"/>
       <c r="BC91" t="inlineStr"/>
@@ -22880,4 +22897,1325 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D101"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>SN</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Section</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Term</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Cost Estimation &amp; Optimization</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Actual Cost (AC)</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Actual Cost  is the total cost incurred for work completed on a project at a given point in time. It includes all direct and indirect costs spent on labor, materials, equipment, and other expenses.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Cost Estimation &amp; Optimization</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Aggregated Budget Variance</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Cumulative difference between total budgeted figures and actual results across multiple categories or projects, highlighting overall financial performance deviations within a specific period</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Planning &amp; Monitoring</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Aggregated SPI</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Indication of overall schedule performance at DevCo level</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Development &amp; Construction</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Annual Procurement Plan / Strategy</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>The Procurement Plan is required to be reviewed and updated by the DevCo as a minimum annually and submitted to PIF for approval in accordance with the requirements of the Project Execution Plan.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Authority</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Each development stage requires approval. The Authority is the relevant party responsible for the approval at the relevant stage (e.g. CEO, Founding Board etc.)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Design &amp; Technical</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>BUA</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Built Up Area (BUA) is the total area being developed or constructed. It is the Gross Floor Area (GFA) plus Parking plus any Service Area.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Cost Estimation &amp; Optimization</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Budget Variance (BV)</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Extent of variance in budget</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Cost Estimation &amp; Optimization</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Budget At Completion (BAC)</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>The Budget at Completion (BAC) represents the total budgeted cost for all the work planned for a project</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Cost Estimation &amp; Optimization</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Estimate To Complete (ETC)</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>The estimated cost required to complete the remaining work of a project</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Cost Estimation &amp; Optimization</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Estimate At Completion (EAC)</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Total forecasted cost of the project based on the ongoing </t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Business Plan</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Documentation developed by PIF informing the Vision and key objectives of the project</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Change Management Log</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>A document summarising the status of all proposed and approved Variations</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Change Management Procedure</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Procedural document stipulating the requirements to be met when administering any amendment to a Contract or Project.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Cost Estimate &amp; Optimization</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Contingency Utilization Rate (CUR)</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Percentage of a project’s allocated contingency fund that has been used to address unforeseen costs or risks, reflecting the efficiency of contingency planning and management.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Development &amp; Construction</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Contract Management Policy</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>A policy outlining award and management of contracts between DevCo and Vendors.</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Cost Estimate &amp; Optimization</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Cost Estimate and Optimization (CE&amp;O)</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Technical function which covers cost benchmarks for development of budgets, and cost optimization levers</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Cost Estimate &amp; Optimization</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Cost Report</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>A document provided on an interim basis to inform of the current financial status of a Project</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Design &amp; Technical</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Design and Technical (D&amp;T)</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Technical Function which covers all design-related topics of a project including architecture, engineering, masterplanning, infrastructure and environment &amp; sustainability</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Development &amp; Construction</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Development and Construction (D&amp;C)</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Technical function which covers construction project execution plans, contract management and procurement, and construction quality and Health, Safety and Environment (HSE) topics</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Planning &amp; Monitoring</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Earned Value (EV)</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Value of the work that is completed at a given time, measured against the budgeted cost.</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Planning &amp; Monitoring</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Extension of Time (EOT)</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Extension of Time is a contractual provision in construction allowing the project completion date to be extended due to unforeseen delays beyond the contractor’s control, ensuring fairness and mitigating penalties.</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Design &amp; Technical</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Gross Floor Area (GFA)</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Gross Floor Area (GFA) is the total floor area of a building including any underground saleable or leasable area but excluding parking and underground technical/service areas. The GFA is calculated based on the distance from external wall to external wall.</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Innovation &amp; Technology</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Innovation and Technology (I&amp;T)</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Technical function which covers incorporation of high-impact advanced technologies and methodologies across the entire project life cycle, and implementation of smart city use cases.</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Development &amp; Construction</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Inspection Test Plan (ITP)</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>A document which specifies the manatory Inspection, Witness and Hold Points throughout construction that must be verified by a suitably qualified person before works are authorised to proceed.</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Key Performance Indicator (KPI)</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Key quantifiable indicators of progress toward an intended result</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Development &amp; Construction</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Non-Conformance Report (NCR)</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Non-Conformance Report is a quality management document that identifies, tracks, and records deviations from specified standards, facilitating process improvement and quality control.</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Cost Estimate &amp; Optimization</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Planned Budget (PB)</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> It represents how much is expected to be spent at a given point in time from the Approved Over All Budget (BAC)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Planning &amp; Monitoring</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Planned Value (PV)</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>The amount of work that was planned to be completed at a given time as per the approved Schedule.</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Planning &amp; Monitoring</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Planning and Monitoring (P&amp;M)</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Technical Function which covers schedule development and monitoring, and risk management</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Development &amp; Construction</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Procurement Strategy</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Methodical approach for determining the contractural relationship and agreements between DevCo and Vendors</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Development &amp; Construction</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Procurement Procedures Manual</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>A manual which details every aspect of the tendering and overall procurement activities.</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Development &amp; Construction</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Project Execution Plan (PEP)</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Project Execution Plan prepared initially by PIF as part of the Business Plan Stage, which is then passed to the DevCo to lead, review and update from Masterplan Stage onwards</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Development &amp; Construction</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Request For Information (RFI)</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A formal communication tool for requesing information </t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Development &amp; Construction</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Rework Cost</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Indication of the rework done due to quality, design etc issues</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Planning &amp; Monitoring</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Schedule Performance Index (SPI)</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Indication of project schedule performance</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Cost Estimate &amp; Optimization</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Soft Cost</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Soft costs are indirect, non-physical expenses in a construction project that are not directly tied to labor, materials, or physical construction work.</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Stage</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>The description of the Project Stage as per Development Company and PIF terminology.</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Strategy &amp; Operations</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Strategy &amp; Organization</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Technical Function which covers topics around strategy development and execution, people and tools.</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Design &amp; Technical</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Value Engineering</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Process to derive greater value within a Project seeking improvement in time and/ or cost outcomes</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Development &amp; Construction</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Vendor Database</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>A database of Vendors, including pre-qualified Vendors, Vendor appraisal and performance assessment and a list of blacklisted Vendors.</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr"/>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr"/>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr"/>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr"/>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr"/>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr"/>
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr"/>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr"/>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr"/>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="inlineStr"/>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="inlineStr"/>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="inlineStr"/>
+      <c r="C56" t="inlineStr"/>
+      <c r="D56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="inlineStr"/>
+      <c r="C58" t="inlineStr"/>
+      <c r="D58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="inlineStr"/>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="inlineStr"/>
+      <c r="C60" t="inlineStr"/>
+      <c r="D60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="inlineStr"/>
+      <c r="C61" t="inlineStr"/>
+      <c r="D61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="inlineStr"/>
+      <c r="C62" t="inlineStr"/>
+      <c r="D62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="inlineStr"/>
+      <c r="D63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="inlineStr"/>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="inlineStr"/>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="inlineStr"/>
+      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" t="inlineStr"/>
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="inlineStr"/>
+      <c r="C68" t="inlineStr"/>
+      <c r="D68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" t="inlineStr"/>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr"/>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" t="inlineStr"/>
+      <c r="C70" t="inlineStr"/>
+      <c r="D70" t="inlineStr"/>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" t="inlineStr"/>
+      <c r="C71" t="inlineStr"/>
+      <c r="D71" t="inlineStr"/>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" t="inlineStr"/>
+      <c r="C72" t="inlineStr"/>
+      <c r="D72" t="inlineStr"/>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" t="inlineStr"/>
+      <c r="C73" t="inlineStr"/>
+      <c r="D73" t="inlineStr"/>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" t="inlineStr"/>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" t="inlineStr"/>
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" t="inlineStr"/>
+      <c r="C76" t="inlineStr"/>
+      <c r="D76" t="inlineStr"/>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" t="inlineStr"/>
+      <c r="C77" t="inlineStr"/>
+      <c r="D77" t="inlineStr"/>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" t="inlineStr"/>
+      <c r="C78" t="inlineStr"/>
+      <c r="D78" t="inlineStr"/>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" t="inlineStr"/>
+      <c r="C79" t="inlineStr"/>
+      <c r="D79" t="inlineStr"/>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" t="inlineStr"/>
+      <c r="C80" t="inlineStr"/>
+      <c r="D80" t="inlineStr"/>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" t="inlineStr"/>
+      <c r="C81" t="inlineStr"/>
+      <c r="D81" t="inlineStr"/>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>81</v>
+      </c>
+      <c r="B82" t="inlineStr"/>
+      <c r="C82" t="inlineStr"/>
+      <c r="D82" t="inlineStr"/>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>82</v>
+      </c>
+      <c r="B83" t="inlineStr"/>
+      <c r="C83" t="inlineStr"/>
+      <c r="D83" t="inlineStr"/>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>83</v>
+      </c>
+      <c r="B84" t="inlineStr"/>
+      <c r="C84" t="inlineStr"/>
+      <c r="D84" t="inlineStr"/>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>84</v>
+      </c>
+      <c r="B85" t="inlineStr"/>
+      <c r="C85" t="inlineStr"/>
+      <c r="D85" t="inlineStr"/>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" t="inlineStr"/>
+      <c r="C86" t="inlineStr"/>
+      <c r="D86" t="inlineStr"/>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>86</v>
+      </c>
+      <c r="B87" t="inlineStr"/>
+      <c r="C87" t="inlineStr"/>
+      <c r="D87" t="inlineStr"/>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>87</v>
+      </c>
+      <c r="B88" t="inlineStr"/>
+      <c r="C88" t="inlineStr"/>
+      <c r="D88" t="inlineStr"/>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>88</v>
+      </c>
+      <c r="B89" t="inlineStr"/>
+      <c r="C89" t="inlineStr"/>
+      <c r="D89" t="inlineStr"/>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" t="inlineStr"/>
+      <c r="C90" t="inlineStr"/>
+      <c r="D90" t="inlineStr"/>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>90</v>
+      </c>
+      <c r="B91" t="inlineStr"/>
+      <c r="C91" t="inlineStr"/>
+      <c r="D91" t="inlineStr"/>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>91</v>
+      </c>
+      <c r="B92" t="inlineStr"/>
+      <c r="C92" t="inlineStr"/>
+      <c r="D92" t="inlineStr"/>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>92</v>
+      </c>
+      <c r="B93" t="inlineStr"/>
+      <c r="C93" t="inlineStr"/>
+      <c r="D93" t="inlineStr"/>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>93</v>
+      </c>
+      <c r="B94" t="inlineStr"/>
+      <c r="C94" t="inlineStr"/>
+      <c r="D94" t="inlineStr"/>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>94</v>
+      </c>
+      <c r="B95" t="inlineStr"/>
+      <c r="C95" t="inlineStr"/>
+      <c r="D95" t="inlineStr"/>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>95</v>
+      </c>
+      <c r="B96" t="inlineStr"/>
+      <c r="C96" t="inlineStr"/>
+      <c r="D96" t="inlineStr"/>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>96</v>
+      </c>
+      <c r="B97" t="inlineStr"/>
+      <c r="C97" t="inlineStr"/>
+      <c r="D97" t="inlineStr"/>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>97</v>
+      </c>
+      <c r="B98" t="inlineStr"/>
+      <c r="C98" t="inlineStr"/>
+      <c r="D98" t="inlineStr"/>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>98</v>
+      </c>
+      <c r="B99" t="inlineStr"/>
+      <c r="C99" t="inlineStr"/>
+      <c r="D99" t="inlineStr"/>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>99</v>
+      </c>
+      <c r="B100" t="inlineStr"/>
+      <c r="C100" t="inlineStr"/>
+      <c r="D100" t="inlineStr"/>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>100</v>
+      </c>
+      <c r="B101" t="inlineStr"/>
+      <c r="C101" t="inlineStr"/>
+      <c r="D101" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated with org chart
</commit_message>
<xml_diff>
--- a/master_sheet.xlsx
+++ b/master_sheet.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Glossary" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="OrgChart" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -31537,7 +31538,7 @@
       <c r="CL202" t="inlineStr"/>
       <c r="CM202" t="inlineStr"/>
       <c r="CN202" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="CO202" t="n">
         <v>2</v>
@@ -31821,7 +31822,7 @@
       <c r="CL203" t="inlineStr"/>
       <c r="CM203" t="inlineStr"/>
       <c r="CN203" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="CO203" t="n">
         <v>2</v>
@@ -32105,7 +32106,7 @@
       <c r="CL204" t="inlineStr"/>
       <c r="CM204" t="inlineStr"/>
       <c r="CN204" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="CO204" t="n">
         <v>2</v>
@@ -32377,7 +32378,7 @@
       <c r="CL205" t="inlineStr"/>
       <c r="CM205" t="inlineStr"/>
       <c r="CN205" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="CO205" t="n">
         <v>3</v>
@@ -32681,7 +32682,7 @@
       <c r="CL206" t="inlineStr"/>
       <c r="CM206" t="inlineStr"/>
       <c r="CN206" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="CO206" t="n">
         <v>3</v>
@@ -32945,7 +32946,7 @@
       <c r="CL207" t="inlineStr"/>
       <c r="CM207" t="inlineStr"/>
       <c r="CN207" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="CO207" t="n">
         <v>3</v>
@@ -33201,7 +33202,7 @@
       <c r="CL208" t="inlineStr"/>
       <c r="CM208" t="inlineStr"/>
       <c r="CN208" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="CO208" t="n">
         <v>3</v>
@@ -59848,4 +59849,695 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>DevCo</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>EmployeeID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Group</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Label</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ManagerID</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Sub-Label</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Diriyah</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Filled</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Chief Development Officer</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>CDO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Diriyah</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Filled</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Head</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Development</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Diriyah</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Filled</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Head</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Projects</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Diriyah</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Filled</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Head</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Masterplan</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Diriyah</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Missing</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>HSE</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>HSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Diriyah</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Filled</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Chief Devt</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>MP1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Diriyah</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Filled</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Chief Devt</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>MP2</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Diriyah</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Vacant</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Chief Devt</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>MP3</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Diriyah</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Vacant</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Project Lead</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>3</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>MP1</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Diriyah</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>10</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Filled</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Project Lead</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>3</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>MP2</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Diriyah</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>11</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Filled</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Project Lead</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>3</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>MP3</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Diriyah</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>12</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Missing</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Lead</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>3</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Stakeholder Interface</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Qiddiya</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Filled</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Chief Development Officer</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>CDO</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Qiddiya</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Filled</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Head</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Development</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Qiddiya</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>3</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Filled</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Head</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Projects</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Qiddiya</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>4</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Filled</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Head</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Masterplan</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Qiddiya</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>5</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Vacant</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Chief Devt</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>2</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>MP1</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Qiddiya</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>6</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Vacant</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Chief Devt</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>2</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>MP2</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Qiddiya</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>7</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Vacant</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Chief Devt</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>MP3</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Qiddiya</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>8</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Vacant</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Project Lead</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>3</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>MP1</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Qiddiya</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>9</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Filled</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Project Lead</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>3</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>MP2</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Qiddiya</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>10</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Filled</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Project Lead</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>3</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>MP3</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Qiddiya</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>11</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Missing</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Lead</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>3</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Stakeholder Interface</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>